<commit_message>
location bulk issue resolved
</commit_message>
<xml_diff>
--- a/src/temp/temp.xlsx
+++ b/src/temp/temp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivsharma\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35619FE1-5062-4523-A1BF-EB85C7C7BCAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE457B3-F1DA-44CF-9A8A-69B0DA6FE84A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,27 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Python</t>
+    <t>delhi</t>
   </si>
   <si>
-    <t>JavaScript</t>
-  </si>
-  <si>
-    <t>React Js</t>
-  </si>
-  <si>
-    <t>css</t>
-  </si>
-  <si>
-    <t>html</t>
-  </si>
-  <si>
-    <t>angular</t>
+    <t>jaipur J</t>
   </si>
 </sst>
 </file>
@@ -415,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -433,29 +421,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
type resolved for lowercase
</commit_message>
<xml_diff>
--- a/src/temp/temp.xlsx
+++ b/src/temp/temp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivsharma\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE457B3-F1DA-44CF-9A8A-69B0DA6FE84A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBD663C-4B65-4067-A2F6-4C7B0386AD23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Name</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>jaipur J</t>
+  </si>
+  <si>
+    <t>Gurgain</t>
   </si>
 </sst>
 </file>
@@ -403,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -421,9 +424,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>